<commit_message>
scraped two more papers
</commit_message>
<xml_diff>
--- a/data/oegres_AZ/oegres_AZ.xlsx
+++ b/data/oegres_AZ/oegres_AZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alina\Documents\git\oegres\data\oegres_AZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B80E7B-769F-4400-AEDC-E8820C5561E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43463F5-41D5-4F8E-8E41-383A7E0BE606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15279" uniqueCount="1288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16069" uniqueCount="1299">
   <si>
     <t>datasetID</t>
   </si>
@@ -3918,6 +3918,39 @@
   </si>
   <si>
     <t>imbibition and chilling</t>
+  </si>
+  <si>
+    <t>negundo</t>
+  </si>
+  <si>
+    <t>Yekaterinburg</t>
+  </si>
+  <si>
+    <t>18-23</t>
+  </si>
+  <si>
+    <t>figure 3</t>
+  </si>
+  <si>
+    <t>small seed box 1</t>
+  </si>
+  <si>
+    <t>small seed box 2</t>
+  </si>
+  <si>
+    <t>small seed box 3</t>
+  </si>
+  <si>
+    <t>ginnala</t>
+  </si>
+  <si>
+    <t>big seed box 1</t>
+  </si>
+  <si>
+    <t>big seed box 2</t>
+  </si>
+  <si>
+    <t>big seed box 3</t>
   </si>
 </sst>
 </file>
@@ -4073,7 +4106,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4265,6 +4298,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -4426,7 +4465,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4469,6 +4508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4860,8 +4900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -13692,11 +13732,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF879E8-8D94-46F6-B2BF-DB1D9526E866}">
-  <dimension ref="A1:AT497"/>
+  <dimension ref="A1:AT530"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P488" sqref="P488"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -54768,7 +54808,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="481" spans="1:44" x14ac:dyDescent="0.6">
+    <row r="481" spans="1:45" x14ac:dyDescent="0.6">
       <c r="A481" s="28" t="s">
         <v>1270</v>
       </c>
@@ -54871,7 +54911,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="482" spans="1:44" x14ac:dyDescent="0.6">
+    <row r="482" spans="1:45" x14ac:dyDescent="0.6">
       <c r="A482" s="28" t="s">
         <v>1270</v>
       </c>
@@ -54974,7 +55014,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="483" spans="1:44" x14ac:dyDescent="0.6">
+    <row r="483" spans="1:45" x14ac:dyDescent="0.6">
       <c r="A483" s="28" t="s">
         <v>1270</v>
       </c>
@@ -55077,7 +55117,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="484" spans="1:44" x14ac:dyDescent="0.6">
+    <row r="484" spans="1:45" x14ac:dyDescent="0.6">
       <c r="A484" s="28" t="s">
         <v>1270</v>
       </c>
@@ -55180,7 +55220,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="485" spans="1:44" x14ac:dyDescent="0.6">
+    <row r="485" spans="1:45" x14ac:dyDescent="0.6">
       <c r="A485" s="28" t="s">
         <v>1270</v>
       </c>
@@ -55283,7 +55323,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="486" spans="1:44" x14ac:dyDescent="0.6">
+    <row r="486" spans="1:45" x14ac:dyDescent="0.6">
       <c r="A486" s="28" t="s">
         <v>1270</v>
       </c>
@@ -55386,7 +55426,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="487" spans="1:44" x14ac:dyDescent="0.6">
+    <row r="487" spans="1:45" x14ac:dyDescent="0.6">
       <c r="A487" s="28" t="s">
         <v>1270</v>
       </c>
@@ -55489,17 +55529,3777 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="488" spans="1:44" x14ac:dyDescent="0.6">
-      <c r="Z488" s="28"/>
-      <c r="AD488" s="28"/>
-    </row>
-    <row r="492" spans="1:44" x14ac:dyDescent="0.6">
-      <c r="A492" t="s">
+    <row r="488" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A488" t="s">
         <v>1271</v>
       </c>
-    </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.6">
-      <c r="A497" t="s">
+      <c r="B488" t="s">
+        <v>37</v>
+      </c>
+      <c r="C488" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D488" t="s">
+        <v>621</v>
+      </c>
+      <c r="E488" t="s">
+        <v>1288</v>
+      </c>
+      <c r="G488" t="s">
+        <v>47</v>
+      </c>
+      <c r="H488" t="s">
+        <v>42</v>
+      </c>
+      <c r="I488" t="s">
+        <v>1289</v>
+      </c>
+      <c r="M488" t="s">
+        <v>1278</v>
+      </c>
+      <c r="O488">
+        <v>2018</v>
+      </c>
+      <c r="Q488" t="s">
+        <v>156</v>
+      </c>
+      <c r="R488">
+        <v>5</v>
+      </c>
+      <c r="T488">
+        <v>20</v>
+      </c>
+      <c r="U488" t="s">
+        <v>64</v>
+      </c>
+      <c r="X488" s="11" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Z488">
+        <v>10</v>
+      </c>
+      <c r="AD488" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF488" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI488" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ488" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK488">
+        <v>0</v>
+      </c>
+      <c r="AL488" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP488">
+        <v>20</v>
+      </c>
+      <c r="AR488" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS488" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="489" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A489" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B489" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C489" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D489" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E489" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F489" s="28"/>
+      <c r="G489" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H489" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I489" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J489" s="28"/>
+      <c r="K489" s="28"/>
+      <c r="L489" s="28"/>
+      <c r="M489" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N489" s="28"/>
+      <c r="O489" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P489" s="28"/>
+      <c r="Q489" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R489" s="28">
+        <v>5</v>
+      </c>
+      <c r="T489" s="28">
+        <v>20</v>
+      </c>
+      <c r="U489" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="V489" s="24"/>
+      <c r="W489" s="28"/>
+      <c r="X489" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y489" s="28"/>
+      <c r="Z489" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA489" s="28"/>
+      <c r="AB489" s="28"/>
+      <c r="AC489" s="28"/>
+      <c r="AD489" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE489" s="28"/>
+      <c r="AF489" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG489" s="28"/>
+      <c r="AH489" s="28"/>
+      <c r="AI489" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ489" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK489" s="28">
+        <v>0</v>
+      </c>
+      <c r="AL489" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP489" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ489" s="28"/>
+      <c r="AR489" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS489" s="28" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="490" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A490" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B490" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C490" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D490" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E490" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F490" s="28"/>
+      <c r="G490" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H490" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I490" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J490" s="28"/>
+      <c r="K490" s="28"/>
+      <c r="L490" s="28"/>
+      <c r="M490" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N490" s="28"/>
+      <c r="O490" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P490" s="28"/>
+      <c r="Q490" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R490" s="28">
+        <v>5</v>
+      </c>
+      <c r="T490" s="28">
+        <v>20</v>
+      </c>
+      <c r="U490" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="V490" s="24"/>
+      <c r="W490" s="28"/>
+      <c r="X490" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y490" s="28"/>
+      <c r="Z490" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA490" s="28"/>
+      <c r="AB490" s="28"/>
+      <c r="AC490" s="28"/>
+      <c r="AD490" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE490" s="28"/>
+      <c r="AF490" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG490" s="28"/>
+      <c r="AH490" s="28"/>
+      <c r="AI490" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ490" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK490" s="28">
+        <v>0</v>
+      </c>
+      <c r="AL490" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP490" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ490" s="28"/>
+      <c r="AR490" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS490" s="28" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="491" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A491" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B491" s="28" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C491" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D491" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E491" s="28" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F491" s="28"/>
+      <c r="G491" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H491" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I491" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J491" s="28"/>
+      <c r="K491" s="28"/>
+      <c r="L491" s="28"/>
+      <c r="M491" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N491" s="28"/>
+      <c r="O491" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P491" s="28"/>
+      <c r="Q491" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R491" s="28">
+        <v>5</v>
+      </c>
+      <c r="S491" s="28"/>
+      <c r="T491" s="28">
+        <v>20</v>
+      </c>
+      <c r="U491" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="X491" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Z491" s="28">
+        <v>10</v>
+      </c>
+      <c r="AD491" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE491" s="28"/>
+      <c r="AF491" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG491" s="28"/>
+      <c r="AH491" s="28"/>
+      <c r="AI491" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ491" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK491" s="28">
+        <v>0</v>
+      </c>
+      <c r="AL491" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP491" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ491" s="28"/>
+      <c r="AR491" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS491" s="28" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="492" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A492" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B492" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C492" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D492" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E492" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F492" s="28"/>
+      <c r="G492" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H492" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I492" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J492" s="28"/>
+      <c r="K492" s="28"/>
+      <c r="L492" s="28"/>
+      <c r="M492" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N492" s="28"/>
+      <c r="O492" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P492" s="28"/>
+      <c r="Q492" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R492" s="28">
+        <v>5</v>
+      </c>
+      <c r="S492" s="28"/>
+      <c r="T492" s="28">
+        <v>20</v>
+      </c>
+      <c r="U492" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V492" s="24"/>
+      <c r="W492" s="28"/>
+      <c r="X492" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y492" s="28"/>
+      <c r="Z492" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC492">
+        <v>30</v>
+      </c>
+      <c r="AD492" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE492" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF492" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI492" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ492" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK492">
+        <v>0</v>
+      </c>
+      <c r="AL492" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP492">
+        <v>20</v>
+      </c>
+      <c r="AR492" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS492" s="28" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="493" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A493" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B493" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C493" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D493" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E493" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F493" s="28"/>
+      <c r="G493" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H493" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I493" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J493" s="28"/>
+      <c r="K493" s="28"/>
+      <c r="L493" s="28"/>
+      <c r="M493" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N493" s="28"/>
+      <c r="O493" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P493" s="28"/>
+      <c r="Q493" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R493" s="28">
+        <v>5</v>
+      </c>
+      <c r="S493" s="28"/>
+      <c r="T493" s="28">
+        <v>20</v>
+      </c>
+      <c r="U493" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V493" s="24"/>
+      <c r="W493" s="28"/>
+      <c r="X493" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y493" s="28"/>
+      <c r="Z493" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC493">
+        <v>60</v>
+      </c>
+      <c r="AD493" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE493" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF493" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI493" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ493" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK493">
+        <v>0</v>
+      </c>
+      <c r="AL493" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP493">
+        <v>20</v>
+      </c>
+      <c r="AR493" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS493" s="28" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="494" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A494" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B494" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C494" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D494" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E494" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F494" s="28"/>
+      <c r="G494" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H494" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I494" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J494" s="28"/>
+      <c r="K494" s="28"/>
+      <c r="L494" s="28"/>
+      <c r="M494" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N494" s="28"/>
+      <c r="O494" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P494" s="28"/>
+      <c r="Q494" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R494" s="28">
+        <v>5</v>
+      </c>
+      <c r="S494" s="28"/>
+      <c r="T494" s="28">
+        <v>20</v>
+      </c>
+      <c r="U494" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V494" s="24"/>
+      <c r="W494" s="28"/>
+      <c r="X494" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y494" s="28"/>
+      <c r="Z494" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC494">
+        <v>90</v>
+      </c>
+      <c r="AD494" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE494" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF494" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI494" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ494" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK494">
+        <v>0</v>
+      </c>
+      <c r="AL494" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP494">
+        <v>20</v>
+      </c>
+      <c r="AR494" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS494" s="28" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="495" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A495" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B495" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C495" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D495" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E495" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F495" s="28"/>
+      <c r="G495" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H495" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I495" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J495" s="28"/>
+      <c r="K495" s="28"/>
+      <c r="L495" s="28"/>
+      <c r="M495" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N495" s="28"/>
+      <c r="O495" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P495" s="28"/>
+      <c r="Q495" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R495" s="28">
+        <v>5</v>
+      </c>
+      <c r="S495" s="28"/>
+      <c r="T495" s="28">
+        <v>20</v>
+      </c>
+      <c r="U495" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V495" s="24"/>
+      <c r="W495" s="28"/>
+      <c r="X495" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y495" s="28"/>
+      <c r="Z495" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC495">
+        <v>120</v>
+      </c>
+      <c r="AD495" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE495" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF495" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI495" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ495" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK495">
+        <v>12.865</v>
+      </c>
+      <c r="AL495" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP495" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ495" s="28"/>
+      <c r="AR495" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS495" s="28" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="496" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A496" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B496" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C496" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D496" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E496" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F496" s="28"/>
+      <c r="G496" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H496" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I496" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J496" s="28"/>
+      <c r="K496" s="28"/>
+      <c r="L496" s="28"/>
+      <c r="M496" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N496" s="28"/>
+      <c r="O496" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P496" s="28"/>
+      <c r="Q496" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R496" s="28">
+        <v>5</v>
+      </c>
+      <c r="S496" s="28"/>
+      <c r="T496" s="28">
+        <v>20</v>
+      </c>
+      <c r="U496" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V496" s="24"/>
+      <c r="W496" s="28"/>
+      <c r="X496" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y496" s="28"/>
+      <c r="Z496" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC496" s="28">
+        <v>30</v>
+      </c>
+      <c r="AD496" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE496" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF496" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI496" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ496" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK496">
+        <v>0</v>
+      </c>
+      <c r="AL496" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP496" s="28">
+        <v>20</v>
+      </c>
+      <c r="AR496" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS496" s="28" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="497" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A497" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B497" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C497" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D497" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E497" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F497" s="28"/>
+      <c r="G497" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H497" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I497" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J497" s="28"/>
+      <c r="K497" s="28"/>
+      <c r="L497" s="28"/>
+      <c r="M497" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N497" s="28"/>
+      <c r="O497" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P497" s="28"/>
+      <c r="Q497" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R497" s="28">
+        <v>5</v>
+      </c>
+      <c r="S497" s="28"/>
+      <c r="T497" s="28">
+        <v>20</v>
+      </c>
+      <c r="U497" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V497" s="24"/>
+      <c r="W497" s="28"/>
+      <c r="X497" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y497" s="28"/>
+      <c r="Z497" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC497" s="28">
+        <v>60</v>
+      </c>
+      <c r="AD497" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE497" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF497" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI497" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ497" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK497">
+        <v>0</v>
+      </c>
+      <c r="AL497" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP497" s="28">
+        <v>20</v>
+      </c>
+      <c r="AR497" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS497" s="28" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="498" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A498" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B498" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C498" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D498" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E498" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F498" s="28"/>
+      <c r="G498" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H498" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I498" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J498" s="28"/>
+      <c r="K498" s="28"/>
+      <c r="L498" s="28"/>
+      <c r="M498" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N498" s="28"/>
+      <c r="O498" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P498" s="28"/>
+      <c r="Q498" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R498" s="28">
+        <v>5</v>
+      </c>
+      <c r="S498" s="28"/>
+      <c r="T498" s="28">
+        <v>20</v>
+      </c>
+      <c r="U498" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V498" s="24"/>
+      <c r="W498" s="28"/>
+      <c r="X498" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y498" s="28"/>
+      <c r="Z498" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC498" s="28">
+        <v>90</v>
+      </c>
+      <c r="AD498" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE498" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF498" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI498" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ498" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK498" s="28">
+        <v>4.101</v>
+      </c>
+      <c r="AL498" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP498" s="28">
+        <v>20</v>
+      </c>
+      <c r="AR498" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS498" s="28" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="499" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A499" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B499" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C499" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D499" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E499" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F499" s="28"/>
+      <c r="G499" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H499" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I499" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J499" s="28"/>
+      <c r="K499" s="28"/>
+      <c r="L499" s="28"/>
+      <c r="M499" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N499" s="28"/>
+      <c r="O499" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P499" s="28"/>
+      <c r="Q499" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R499" s="28">
+        <v>5</v>
+      </c>
+      <c r="S499" s="28"/>
+      <c r="T499" s="28">
+        <v>20</v>
+      </c>
+      <c r="U499" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V499" s="24"/>
+      <c r="W499" s="28"/>
+      <c r="X499" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y499" s="28"/>
+      <c r="Z499" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC499" s="28">
+        <v>120</v>
+      </c>
+      <c r="AD499" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE499" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF499" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI499" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ499" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK499" s="28">
+        <v>10.169</v>
+      </c>
+      <c r="AL499" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP499" s="28">
+        <v>20</v>
+      </c>
+      <c r="AR499" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS499" s="28" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="500" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A500" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B500" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C500" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D500" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E500" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F500" s="28"/>
+      <c r="G500" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H500" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I500" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J500" s="28"/>
+      <c r="K500" s="28"/>
+      <c r="L500" s="28"/>
+      <c r="M500" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N500" s="28"/>
+      <c r="O500" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P500" s="28"/>
+      <c r="Q500" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R500" s="28">
+        <v>5</v>
+      </c>
+      <c r="S500" s="28"/>
+      <c r="T500" s="28">
+        <v>20</v>
+      </c>
+      <c r="U500" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V500" s="24"/>
+      <c r="W500" s="28"/>
+      <c r="X500" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y500" s="28"/>
+      <c r="Z500" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC500" s="28">
+        <v>30</v>
+      </c>
+      <c r="AD500" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE500" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF500" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG500" s="28"/>
+      <c r="AH500" s="28"/>
+      <c r="AI500" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ500" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK500">
+        <v>0</v>
+      </c>
+      <c r="AL500" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP500" s="28">
+        <v>20</v>
+      </c>
+      <c r="AR500" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS500" s="28" t="s">
+        <v>1294</v>
+      </c>
+      <c r="AT500" s="28"/>
+    </row>
+    <row r="501" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A501" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B501" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C501" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D501" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E501" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F501" s="28"/>
+      <c r="G501" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H501" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I501" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J501" s="28"/>
+      <c r="K501" s="28"/>
+      <c r="L501" s="28"/>
+      <c r="M501" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N501" s="28"/>
+      <c r="O501" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P501" s="28"/>
+      <c r="Q501" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R501" s="28">
+        <v>5</v>
+      </c>
+      <c r="S501" s="28"/>
+      <c r="T501" s="28">
+        <v>20</v>
+      </c>
+      <c r="U501" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V501" s="24"/>
+      <c r="W501" s="28"/>
+      <c r="X501" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y501" s="28"/>
+      <c r="Z501" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC501" s="28">
+        <v>60</v>
+      </c>
+      <c r="AD501" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE501" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF501" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG501" s="28"/>
+      <c r="AH501" s="28"/>
+      <c r="AI501" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ501" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK501">
+        <v>2.0790000000000002</v>
+      </c>
+      <c r="AL501" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP501" s="28">
+        <v>20</v>
+      </c>
+      <c r="AR501" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS501" s="28" t="s">
+        <v>1294</v>
+      </c>
+      <c r="AT501" s="28"/>
+    </row>
+    <row r="502" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A502" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B502" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C502" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D502" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E502" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F502" s="28"/>
+      <c r="G502" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H502" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I502" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J502" s="28"/>
+      <c r="K502" s="28"/>
+      <c r="L502" s="28"/>
+      <c r="M502" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N502" s="28"/>
+      <c r="O502" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P502" s="28"/>
+      <c r="Q502" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R502" s="28">
+        <v>5</v>
+      </c>
+      <c r="S502" s="28"/>
+      <c r="T502" s="28">
+        <v>20</v>
+      </c>
+      <c r="U502" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V502" s="24"/>
+      <c r="W502" s="28"/>
+      <c r="X502" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y502" s="28"/>
+      <c r="Z502" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC502" s="28">
+        <v>90</v>
+      </c>
+      <c r="AD502" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE502" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF502" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG502" s="28"/>
+      <c r="AH502" s="28"/>
+      <c r="AI502" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ502" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK502">
+        <v>5.4489999999999998</v>
+      </c>
+      <c r="AL502" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP502" s="28">
+        <v>20</v>
+      </c>
+      <c r="AR502" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS502" s="28" t="s">
+        <v>1294</v>
+      </c>
+      <c r="AT502" s="28"/>
+    </row>
+    <row r="503" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A503" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B503" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C503" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D503" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E503" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F503" s="28"/>
+      <c r="G503" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H503" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I503" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J503" s="28"/>
+      <c r="K503" s="28"/>
+      <c r="L503" s="28"/>
+      <c r="M503" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N503" s="28"/>
+      <c r="O503" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P503" s="28"/>
+      <c r="Q503" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R503" s="28">
+        <v>5</v>
+      </c>
+      <c r="S503" s="28"/>
+      <c r="T503" s="28">
+        <v>20</v>
+      </c>
+      <c r="U503" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V503" s="24"/>
+      <c r="W503" s="28"/>
+      <c r="X503" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y503" s="28"/>
+      <c r="Z503" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC503" s="28">
+        <v>120</v>
+      </c>
+      <c r="AD503" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE503" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF503" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG503" s="28"/>
+      <c r="AH503" s="28"/>
+      <c r="AI503" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ503" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK503">
+        <v>13.989000000000001</v>
+      </c>
+      <c r="AL503" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP503" s="28">
+        <v>20</v>
+      </c>
+      <c r="AR503" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS503" s="28" t="s">
+        <v>1294</v>
+      </c>
+      <c r="AT503" s="28"/>
+    </row>
+    <row r="504" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A504" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B504" s="28" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C504" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D504" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E504" s="28" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F504" s="28"/>
+      <c r="G504" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H504" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I504" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J504" s="28"/>
+      <c r="K504" s="28"/>
+      <c r="L504" s="28"/>
+      <c r="M504" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N504" s="28"/>
+      <c r="O504" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P504" s="28"/>
+      <c r="Q504" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R504" s="28">
+        <v>5</v>
+      </c>
+      <c r="S504" s="28"/>
+      <c r="T504" s="28">
+        <v>20</v>
+      </c>
+      <c r="U504" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="X504" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y504" s="28"/>
+      <c r="Z504" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA504" s="28"/>
+      <c r="AC504" s="28">
+        <v>30</v>
+      </c>
+      <c r="AE504" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF504" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI504" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ504" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK504" s="28">
+        <v>0</v>
+      </c>
+      <c r="AL504" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP504" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ504" s="28"/>
+      <c r="AR504" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS504" s="28" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="505" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A505" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B505" s="28" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C505" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D505" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E505" s="28" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F505" s="28"/>
+      <c r="G505" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H505" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I505" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J505" s="28"/>
+      <c r="K505" s="28"/>
+      <c r="L505" s="28"/>
+      <c r="M505" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N505" s="28"/>
+      <c r="O505" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P505" s="28"/>
+      <c r="Q505" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R505" s="28">
+        <v>5</v>
+      </c>
+      <c r="S505" s="28"/>
+      <c r="T505" s="28">
+        <v>20</v>
+      </c>
+      <c r="U505" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="X505" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y505" s="28"/>
+      <c r="Z505" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA505" s="28"/>
+      <c r="AC505" s="28">
+        <v>60</v>
+      </c>
+      <c r="AE505" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF505" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI505" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ505" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK505">
+        <v>0</v>
+      </c>
+      <c r="AL505" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP505" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ505" s="28"/>
+      <c r="AR505" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS505" s="28" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="506" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A506" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B506" s="28" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C506" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D506" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E506" s="28" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F506" s="28"/>
+      <c r="G506" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H506" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I506" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J506" s="28"/>
+      <c r="K506" s="28"/>
+      <c r="L506" s="28"/>
+      <c r="M506" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N506" s="28"/>
+      <c r="O506" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P506" s="28"/>
+      <c r="Q506" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R506" s="28">
+        <v>5</v>
+      </c>
+      <c r="S506" s="28"/>
+      <c r="T506" s="28">
+        <v>20</v>
+      </c>
+      <c r="U506" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="X506" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y506" s="28"/>
+      <c r="Z506" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA506" s="28"/>
+      <c r="AC506" s="28">
+        <v>90</v>
+      </c>
+      <c r="AE506" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF506" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI506" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ506" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK506" s="30"/>
+      <c r="AL506" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP506" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ506" s="28"/>
+      <c r="AR506" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS506" s="28" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="507" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A507" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B507" s="28" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C507" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D507" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E507" s="28" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F507" s="28"/>
+      <c r="G507" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H507" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I507" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J507" s="28"/>
+      <c r="K507" s="28"/>
+      <c r="L507" s="28"/>
+      <c r="M507" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N507" s="28"/>
+      <c r="O507" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P507" s="28"/>
+      <c r="Q507" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R507" s="28">
+        <v>5</v>
+      </c>
+      <c r="S507" s="28"/>
+      <c r="T507" s="28">
+        <v>20</v>
+      </c>
+      <c r="U507" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="X507" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y507" s="28"/>
+      <c r="Z507" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA507" s="28"/>
+      <c r="AC507" s="28">
+        <v>120</v>
+      </c>
+      <c r="AE507" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF507" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI507" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ507" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK507" s="30"/>
+      <c r="AL507" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP507" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ507" s="28"/>
+      <c r="AR507" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS507" s="28" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="508" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A508" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B508" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C508" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D508" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E508" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="G508" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H508" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I508" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J508" s="28"/>
+      <c r="K508" s="28"/>
+      <c r="L508" s="28"/>
+      <c r="M508" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N508" s="28"/>
+      <c r="O508" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P508" s="28"/>
+      <c r="Q508" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R508" s="28">
+        <v>5</v>
+      </c>
+      <c r="T508" s="28">
+        <v>20</v>
+      </c>
+      <c r="U508" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="X508" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y508" s="28"/>
+      <c r="Z508" s="28">
+        <v>10</v>
+      </c>
+      <c r="AD508" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF508" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG508" s="28"/>
+      <c r="AH508" s="28"/>
+      <c r="AI508" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ508" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK508" s="28">
+        <v>0</v>
+      </c>
+      <c r="AL508" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP508" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ508" s="28"/>
+      <c r="AR508" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS508" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="509" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A509" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B509" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C509" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D509" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E509" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="G509" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H509" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I509" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J509" s="28"/>
+      <c r="K509" s="28"/>
+      <c r="L509" s="28"/>
+      <c r="M509" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N509" s="28"/>
+      <c r="O509" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P509" s="28"/>
+      <c r="Q509" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R509" s="28">
+        <v>5</v>
+      </c>
+      <c r="T509" s="28">
+        <v>20</v>
+      </c>
+      <c r="U509" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="X509" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y509" s="28"/>
+      <c r="Z509" s="28">
+        <v>10</v>
+      </c>
+      <c r="AD509" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF509" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG509" s="28"/>
+      <c r="AH509" s="28"/>
+      <c r="AI509" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ509" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK509" s="28">
+        <v>0</v>
+      </c>
+      <c r="AL509" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP509" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ509" s="28"/>
+      <c r="AR509" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS509" s="28" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="510" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A510" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B510" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C510" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D510" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E510" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="G510" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H510" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I510" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J510" s="28"/>
+      <c r="K510" s="28"/>
+      <c r="L510" s="28"/>
+      <c r="M510" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N510" s="28"/>
+      <c r="O510" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P510" s="28"/>
+      <c r="Q510" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R510" s="28">
+        <v>5</v>
+      </c>
+      <c r="T510" s="28">
+        <v>20</v>
+      </c>
+      <c r="U510" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="X510" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y510" s="28"/>
+      <c r="Z510" s="28">
+        <v>10</v>
+      </c>
+      <c r="AD510" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF510" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG510" s="28"/>
+      <c r="AH510" s="28"/>
+      <c r="AI510" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ510" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK510" s="28">
+        <v>0</v>
+      </c>
+      <c r="AL510" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP510" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ510" s="28"/>
+      <c r="AR510" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS510" s="28" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="511" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A511" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B511" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C511" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D511" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E511" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F511" s="28"/>
+      <c r="G511" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H511" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I511" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J511" s="28"/>
+      <c r="K511" s="28"/>
+      <c r="L511" s="28"/>
+      <c r="M511" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N511" s="28"/>
+      <c r="O511" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P511" s="28"/>
+      <c r="Q511" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R511" s="28">
+        <v>5</v>
+      </c>
+      <c r="S511" s="28"/>
+      <c r="T511" s="28">
+        <v>20</v>
+      </c>
+      <c r="U511" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V511" s="24"/>
+      <c r="W511" s="28"/>
+      <c r="X511" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y511" s="28"/>
+      <c r="Z511" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA511" s="28"/>
+      <c r="AC511" s="28">
+        <v>30</v>
+      </c>
+      <c r="AE511" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF511" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG511" s="28"/>
+      <c r="AH511" s="28"/>
+      <c r="AI511" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ511" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK511" s="28">
+        <v>0</v>
+      </c>
+      <c r="AL511" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP511" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ511" s="28"/>
+      <c r="AR511" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS511" s="28" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="512" spans="1:46" x14ac:dyDescent="0.6">
+      <c r="A512" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B512" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C512" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D512" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E512" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F512" s="28"/>
+      <c r="G512" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H512" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I512" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J512" s="28"/>
+      <c r="K512" s="28"/>
+      <c r="L512" s="28"/>
+      <c r="M512" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N512" s="28"/>
+      <c r="O512" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P512" s="28"/>
+      <c r="Q512" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R512" s="28">
+        <v>5</v>
+      </c>
+      <c r="S512" s="28"/>
+      <c r="T512" s="28">
+        <v>20</v>
+      </c>
+      <c r="U512" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V512" s="24"/>
+      <c r="W512" s="28"/>
+      <c r="X512" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y512" s="28"/>
+      <c r="Z512" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA512" s="28"/>
+      <c r="AC512" s="28">
+        <v>30</v>
+      </c>
+      <c r="AE512" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF512" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG512" s="28"/>
+      <c r="AH512" s="28"/>
+      <c r="AI512" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ512" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK512">
+        <v>0</v>
+      </c>
+      <c r="AL512" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP512" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ512" s="28"/>
+      <c r="AR512" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS512" s="28" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="513" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A513" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B513" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C513" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D513" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E513" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F513" s="28"/>
+      <c r="G513" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H513" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I513" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J513" s="28"/>
+      <c r="K513" s="28"/>
+      <c r="L513" s="28"/>
+      <c r="M513" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N513" s="28"/>
+      <c r="O513" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P513" s="28"/>
+      <c r="Q513" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R513" s="28">
+        <v>5</v>
+      </c>
+      <c r="S513" s="28"/>
+      <c r="T513" s="28">
+        <v>20</v>
+      </c>
+      <c r="U513" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V513" s="24"/>
+      <c r="W513" s="28"/>
+      <c r="X513" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y513" s="28"/>
+      <c r="Z513" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA513" s="28"/>
+      <c r="AC513" s="28">
+        <v>30</v>
+      </c>
+      <c r="AE513" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF513" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG513" s="28"/>
+      <c r="AH513" s="28"/>
+      <c r="AI513" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ513" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK513">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AL513" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP513" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ513" s="28"/>
+      <c r="AR513" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS513" s="28" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="514" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A514" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B514" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C514" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D514" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E514" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F514" s="28"/>
+      <c r="G514" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H514" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I514" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J514" s="28"/>
+      <c r="K514" s="28"/>
+      <c r="L514" s="28"/>
+      <c r="M514" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N514" s="28"/>
+      <c r="O514" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P514" s="28"/>
+      <c r="Q514" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R514" s="28">
+        <v>5</v>
+      </c>
+      <c r="S514" s="28"/>
+      <c r="T514" s="28">
+        <v>20</v>
+      </c>
+      <c r="U514" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V514" s="24"/>
+      <c r="W514" s="28"/>
+      <c r="X514" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y514" s="28"/>
+      <c r="Z514" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA514" s="28"/>
+      <c r="AC514" s="28">
+        <v>60</v>
+      </c>
+      <c r="AE514" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF514" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG514" s="28"/>
+      <c r="AH514" s="28"/>
+      <c r="AI514" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ514" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK514">
+        <v>4.5510000000000002</v>
+      </c>
+      <c r="AL514" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP514" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ514" s="28"/>
+      <c r="AR514" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS514" s="28" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="515" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A515" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B515" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C515" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D515" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E515" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F515" s="28"/>
+      <c r="G515" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H515" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I515" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J515" s="28"/>
+      <c r="K515" s="28"/>
+      <c r="L515" s="28"/>
+      <c r="M515" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N515" s="28"/>
+      <c r="O515" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P515" s="28"/>
+      <c r="Q515" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R515" s="28">
+        <v>5</v>
+      </c>
+      <c r="S515" s="28"/>
+      <c r="T515" s="28">
+        <v>20</v>
+      </c>
+      <c r="U515" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V515" s="24"/>
+      <c r="W515" s="28"/>
+      <c r="X515" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y515" s="28"/>
+      <c r="Z515" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA515" s="28"/>
+      <c r="AC515" s="28">
+        <v>60</v>
+      </c>
+      <c r="AE515" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF515" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG515" s="28"/>
+      <c r="AH515" s="28"/>
+      <c r="AI515" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ515" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK515">
+        <v>6.3479999999999999</v>
+      </c>
+      <c r="AL515" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP515" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ515" s="28"/>
+      <c r="AR515" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS515" s="28" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="516" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A516" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B516" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C516" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D516" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E516" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F516" s="28"/>
+      <c r="G516" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H516" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I516" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J516" s="28"/>
+      <c r="K516" s="28"/>
+      <c r="L516" s="28"/>
+      <c r="M516" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N516" s="28"/>
+      <c r="O516" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P516" s="28"/>
+      <c r="Q516" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R516" s="28">
+        <v>5</v>
+      </c>
+      <c r="S516" s="28"/>
+      <c r="T516" s="28">
+        <v>20</v>
+      </c>
+      <c r="U516" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V516" s="24"/>
+      <c r="W516" s="28"/>
+      <c r="X516" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y516" s="28"/>
+      <c r="Z516" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA516" s="28"/>
+      <c r="AC516" s="28">
+        <v>60</v>
+      </c>
+      <c r="AE516" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF516" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG516" s="28"/>
+      <c r="AH516" s="28"/>
+      <c r="AI516" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ516" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK516">
+        <v>9.0449999999999999</v>
+      </c>
+      <c r="AL516" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP516" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ516" s="28"/>
+      <c r="AR516" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS516" s="28" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="517" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A517" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B517" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C517" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D517" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E517" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F517" s="28"/>
+      <c r="G517" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H517" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I517" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J517" s="28"/>
+      <c r="K517" s="28"/>
+      <c r="L517" s="28"/>
+      <c r="M517" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N517" s="28"/>
+      <c r="O517" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P517" s="28"/>
+      <c r="Q517" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R517" s="28">
+        <v>5</v>
+      </c>
+      <c r="S517" s="28"/>
+      <c r="T517" s="28">
+        <v>20</v>
+      </c>
+      <c r="U517" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V517" s="24"/>
+      <c r="W517" s="28"/>
+      <c r="X517" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y517" s="28"/>
+      <c r="Z517" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA517" s="28"/>
+      <c r="AC517" s="28">
+        <v>90</v>
+      </c>
+      <c r="AE517" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF517" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG517" s="28"/>
+      <c r="AH517" s="28"/>
+      <c r="AI517" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ517" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK517">
+        <v>19.606999999999999</v>
+      </c>
+      <c r="AL517" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP517" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ517" s="28"/>
+      <c r="AR517" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS517" s="28" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="518" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A518" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B518" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C518" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D518" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E518" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F518" s="28"/>
+      <c r="G518" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H518" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I518" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J518" s="28"/>
+      <c r="K518" s="28"/>
+      <c r="L518" s="28"/>
+      <c r="M518" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N518" s="28"/>
+      <c r="O518" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P518" s="28"/>
+      <c r="Q518" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R518" s="28">
+        <v>5</v>
+      </c>
+      <c r="S518" s="28"/>
+      <c r="T518" s="28">
+        <v>20</v>
+      </c>
+      <c r="U518" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V518" s="24"/>
+      <c r="W518" s="28"/>
+      <c r="X518" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y518" s="28"/>
+      <c r="Z518" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA518" s="28"/>
+      <c r="AC518" s="28">
+        <v>90</v>
+      </c>
+      <c r="AE518" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF518" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG518" s="28"/>
+      <c r="AH518" s="28"/>
+      <c r="AI518" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ518" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK518">
+        <v>28.596</v>
+      </c>
+      <c r="AL518" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP518" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ518" s="28"/>
+      <c r="AR518" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS518" s="28" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="519" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A519" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B519" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C519" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D519" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E519" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F519" s="28"/>
+      <c r="G519" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H519" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I519" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J519" s="28"/>
+      <c r="K519" s="28"/>
+      <c r="L519" s="28"/>
+      <c r="M519" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N519" s="28"/>
+      <c r="O519" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P519" s="28"/>
+      <c r="Q519" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R519" s="28">
+        <v>5</v>
+      </c>
+      <c r="S519" s="28"/>
+      <c r="T519" s="28">
+        <v>20</v>
+      </c>
+      <c r="U519" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V519" s="24"/>
+      <c r="W519" s="28"/>
+      <c r="X519" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y519" s="28"/>
+      <c r="Z519" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA519" s="28"/>
+      <c r="AC519" s="28">
+        <v>90</v>
+      </c>
+      <c r="AE519" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF519" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG519" s="28"/>
+      <c r="AH519" s="28"/>
+      <c r="AI519" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ519" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK519">
+        <v>34.887999999999998</v>
+      </c>
+      <c r="AL519" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP519" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ519" s="28"/>
+      <c r="AR519" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS519" s="28" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="520" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A520" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B520" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C520" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D520" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E520" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F520" s="28"/>
+      <c r="G520" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H520" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I520" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J520" s="28"/>
+      <c r="K520" s="28"/>
+      <c r="L520" s="28"/>
+      <c r="M520" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N520" s="28"/>
+      <c r="O520" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P520" s="28"/>
+      <c r="Q520" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R520" s="28">
+        <v>5</v>
+      </c>
+      <c r="S520" s="28"/>
+      <c r="T520" s="28">
+        <v>20</v>
+      </c>
+      <c r="U520" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V520" s="24"/>
+      <c r="W520" s="28"/>
+      <c r="X520" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y520" s="28"/>
+      <c r="Z520" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA520" s="28"/>
+      <c r="AC520" s="28">
+        <v>120</v>
+      </c>
+      <c r="AE520" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF520" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG520" s="28"/>
+      <c r="AH520" s="28"/>
+      <c r="AI520" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ520" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK520">
+        <v>71.742000000000004</v>
+      </c>
+      <c r="AL520" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP520" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ520" s="28"/>
+      <c r="AR520" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS520" s="28" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="521" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A521" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B521" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C521" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D521" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E521" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F521" s="28"/>
+      <c r="G521" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H521" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I521" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J521" s="28"/>
+      <c r="K521" s="28"/>
+      <c r="L521" s="28"/>
+      <c r="M521" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N521" s="28"/>
+      <c r="O521" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P521" s="28"/>
+      <c r="Q521" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R521" s="28">
+        <v>5</v>
+      </c>
+      <c r="S521" s="28"/>
+      <c r="T521" s="28">
+        <v>20</v>
+      </c>
+      <c r="U521" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V521" s="24"/>
+      <c r="W521" s="28"/>
+      <c r="X521" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y521" s="28"/>
+      <c r="Z521" s="28">
+        <v>10</v>
+      </c>
+      <c r="AA521" s="28"/>
+      <c r="AC521" s="28">
+        <v>120</v>
+      </c>
+      <c r="AE521" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF521" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG521" s="28"/>
+      <c r="AH521" s="28"/>
+      <c r="AI521" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ521" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK521">
+        <v>81.180000000000007</v>
+      </c>
+      <c r="AL521" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP521" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ521" s="28"/>
+      <c r="AR521" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS521" s="28" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="522" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A522" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B522" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C522" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D522" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E522" s="28" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F522" s="28"/>
+      <c r="G522" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H522" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I522" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="J522" s="28"/>
+      <c r="K522" s="28"/>
+      <c r="L522" s="28"/>
+      <c r="M522" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N522" s="28"/>
+      <c r="O522" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P522" s="28"/>
+      <c r="Q522" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R522" s="28">
+        <v>5</v>
+      </c>
+      <c r="S522" s="28"/>
+      <c r="T522" s="28">
+        <v>20</v>
+      </c>
+      <c r="U522" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V522" s="24"/>
+      <c r="W522" s="28"/>
+      <c r="X522" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y522" s="28"/>
+      <c r="Z522" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC522" s="28">
+        <v>120</v>
+      </c>
+      <c r="AE522" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF522" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG522" s="28"/>
+      <c r="AH522" s="28"/>
+      <c r="AI522" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ522" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK522">
+        <v>82.302999999999997</v>
+      </c>
+      <c r="AL522" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP522" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ522" s="28"/>
+      <c r="AR522" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS522" s="28" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="523" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A523" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B523" s="28" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C523" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D523" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E523" s="28" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F523" s="28"/>
+      <c r="G523" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H523" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I523" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="M523" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N523" s="28"/>
+      <c r="O523" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P523" s="28"/>
+      <c r="Q523" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R523" s="28">
+        <v>5</v>
+      </c>
+      <c r="S523" s="28"/>
+      <c r="T523" s="28">
+        <v>20</v>
+      </c>
+      <c r="U523" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V523" s="24"/>
+      <c r="W523" s="28"/>
+      <c r="X523" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y523" s="28"/>
+      <c r="Z523" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC523" s="28">
+        <v>30</v>
+      </c>
+      <c r="AE523" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF523" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG523" s="28"/>
+      <c r="AH523" s="28"/>
+      <c r="AI523" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ523" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK523" s="28">
+        <v>0</v>
+      </c>
+      <c r="AL523" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP523" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ523" s="28"/>
+      <c r="AR523" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS523" s="28" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="524" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A524" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B524" s="28" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C524" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D524" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E524" s="28" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F524" s="28"/>
+      <c r="G524" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H524" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I524" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="M524" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N524" s="28"/>
+      <c r="O524" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P524" s="28"/>
+      <c r="Q524" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R524" s="28">
+        <v>5</v>
+      </c>
+      <c r="S524" s="28"/>
+      <c r="T524" s="28">
+        <v>20</v>
+      </c>
+      <c r="U524" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V524" s="24"/>
+      <c r="W524" s="28"/>
+      <c r="X524" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y524" s="28"/>
+      <c r="Z524" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC524">
+        <v>30</v>
+      </c>
+      <c r="AE524" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF524" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG524" s="28"/>
+      <c r="AH524" s="28"/>
+      <c r="AI524" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ524" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK524" s="28">
+        <v>0</v>
+      </c>
+      <c r="AL524" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP524" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ524" s="28"/>
+      <c r="AR524" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS524" s="28" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="525" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A525" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B525" s="28" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C525" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D525" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E525" s="28" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F525" s="28"/>
+      <c r="G525" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H525" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I525" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="M525" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N525" s="28"/>
+      <c r="O525" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P525" s="28"/>
+      <c r="Q525" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R525" s="28">
+        <v>5</v>
+      </c>
+      <c r="S525" s="28"/>
+      <c r="T525" s="28">
+        <v>20</v>
+      </c>
+      <c r="U525" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V525" s="24"/>
+      <c r="W525" s="28"/>
+      <c r="X525" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y525" s="28"/>
+      <c r="Z525" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC525" s="28">
+        <v>60</v>
+      </c>
+      <c r="AE525" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF525" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG525" s="28"/>
+      <c r="AH525" s="28"/>
+      <c r="AI525" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ525" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK525">
+        <v>2.597</v>
+      </c>
+      <c r="AL525" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP525" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ525" s="28"/>
+      <c r="AR525" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS525" s="28" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="526" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A526" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B526" s="28" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C526" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D526" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E526" s="28" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F526" s="28"/>
+      <c r="G526" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H526" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I526" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="M526" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N526" s="28"/>
+      <c r="O526" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P526" s="28"/>
+      <c r="Q526" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R526" s="28">
+        <v>5</v>
+      </c>
+      <c r="S526" s="28"/>
+      <c r="T526" s="28">
+        <v>20</v>
+      </c>
+      <c r="U526" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V526" s="24"/>
+      <c r="W526" s="28"/>
+      <c r="X526" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y526" s="28"/>
+      <c r="Z526" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC526" s="28">
+        <v>90</v>
+      </c>
+      <c r="AE526" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF526" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG526" s="28"/>
+      <c r="AH526" s="28"/>
+      <c r="AI526" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ526" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK526">
+        <v>1.179</v>
+      </c>
+      <c r="AL526" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP526" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ526" s="28"/>
+      <c r="AR526" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS526" s="28" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="527" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A527" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B527" s="28" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C527" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D527" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E527" s="28" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F527" s="28"/>
+      <c r="G527" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H527" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I527" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="M527" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N527" s="28"/>
+      <c r="O527" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P527" s="28"/>
+      <c r="Q527" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R527" s="28">
+        <v>5</v>
+      </c>
+      <c r="S527" s="28"/>
+      <c r="T527" s="28">
+        <v>20</v>
+      </c>
+      <c r="U527" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V527" s="24"/>
+      <c r="W527" s="28"/>
+      <c r="X527" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y527" s="28"/>
+      <c r="Z527" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC527" s="28">
+        <v>60</v>
+      </c>
+      <c r="AE527" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF527" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG527" s="28"/>
+      <c r="AH527" s="28"/>
+      <c r="AI527" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ527" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK527">
+        <v>7.3970000000000002</v>
+      </c>
+      <c r="AL527" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP527" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ527" s="28"/>
+      <c r="AR527" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS527" s="28" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="528" spans="1:45" x14ac:dyDescent="0.6">
+      <c r="A528" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B528" s="28" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C528" s="28" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D528" s="28" t="s">
+        <v>621</v>
+      </c>
+      <c r="E528" s="28" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F528" s="28"/>
+      <c r="G528" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H528" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="I528" s="28" t="s">
+        <v>1289</v>
+      </c>
+      <c r="M528" s="28" t="s">
+        <v>1278</v>
+      </c>
+      <c r="N528" s="28"/>
+      <c r="O528" s="28">
+        <v>2018</v>
+      </c>
+      <c r="P528" s="28"/>
+      <c r="Q528" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="R528" s="28">
+        <v>5</v>
+      </c>
+      <c r="S528" s="28"/>
+      <c r="T528" s="28">
+        <v>20</v>
+      </c>
+      <c r="U528" s="28" t="s">
+        <v>1252</v>
+      </c>
+      <c r="V528" s="24"/>
+      <c r="W528" s="28"/>
+      <c r="X528" s="24" t="s">
+        <v>1290</v>
+      </c>
+      <c r="Y528" s="28"/>
+      <c r="Z528" s="28">
+        <v>10</v>
+      </c>
+      <c r="AC528" s="28">
+        <v>90</v>
+      </c>
+      <c r="AE528" s="28" t="s">
+        <v>1235</v>
+      </c>
+      <c r="AF528" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG528" s="28"/>
+      <c r="AH528" s="28"/>
+      <c r="AI528" s="28" t="s">
+        <v>1232</v>
+      </c>
+      <c r="AJ528" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK528">
+        <v>17.648</v>
+      </c>
+      <c r="AL528" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP528" s="28">
+        <v>20</v>
+      </c>
+      <c r="AQ528" s="28"/>
+      <c r="AR528" s="28" t="s">
+        <v>1291</v>
+      </c>
+      <c r="AS528" s="28" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="529" spans="1:36" x14ac:dyDescent="0.6">
+      <c r="AE529" s="28"/>
+      <c r="AF529" s="28"/>
+      <c r="AG529" s="28"/>
+      <c r="AH529" s="28"/>
+      <c r="AI529" s="28"/>
+      <c r="AJ529" s="28"/>
+    </row>
+    <row r="530" spans="1:36" x14ac:dyDescent="0.6">
+      <c r="A530" t="s">
         <v>1272</v>
       </c>
     </row>

</xml_diff>